<commit_message>
Begining work to test basic combat and game messages.
</commit_message>
<xml_diff>
--- a/Documentation/Mobs, NPC, Items, mm.xlsx
+++ b/Documentation/Mobs, NPC, Items, mm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="Denne_projektmappe" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Mobs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -74,15 +74,6 @@
   </si>
   <si>
     <t>Human</t>
-  </si>
-  <si>
-    <t>Briggand</t>
-  </si>
-  <si>
-    <t>Club</t>
-  </si>
-  <si>
-    <t>Stun</t>
   </si>
   <si>
     <t>Gold Drop</t>
@@ -213,13 +204,48 @@
   <si>
     <t>The Iron Daggers Head Quarters.</t>
   </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Defence</t>
+  </si>
+  <si>
+    <t>ExpReward</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>knife</t>
+  </si>
+  <si>
+    <t>Steal</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -247,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -256,6 +282,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,68 +618,83 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -668,20 +710,29 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -689,88 +740,101 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
+        <v>66</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10003</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10004</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10005</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10006</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10007</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10008</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10009</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10010</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10011</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10012</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10013</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10014</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10015</v>
       </c>
@@ -997,6 +1061,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1022,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1034,7 +1099,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -1055,16 +1120,16 @@
         <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1358,34 +1423,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1393,22 +1458,22 @@
         <v>30001</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1417,10 +1482,10 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1429,7 +1494,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1437,7 +1502,7 @@
         <v>30003</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1445,7 +1510,7 @@
         <v>30004</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1453,7 +1518,7 @@
         <v>30005</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1461,7 +1526,7 @@
         <v>30006</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1469,7 +1534,7 @@
         <v>30007</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1477,7 +1542,7 @@
         <v>30008</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="13.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1485,7 +1550,7 @@
         <v>30009</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1493,7 +1558,7 @@
         <v>30010</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1501,7 +1566,7 @@
         <v>30011</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1509,7 +1574,7 @@
         <v>30012</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1517,7 +1582,7 @@
         <v>30013</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1525,7 +1590,7 @@
         <v>30014</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1533,7 +1598,7 @@
         <v>30015</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1541,7 +1606,7 @@
         <v>30016</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1549,7 +1614,7 @@
         <v>30017</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1557,7 +1622,7 @@
         <v>30018</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1565,7 +1630,7 @@
         <v>30019</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1638,7 @@
         <v>30020</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1646,7 @@
         <v>30021</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1589,7 +1654,7 @@
         <v>30022</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1597,7 +1662,7 @@
         <v>30023</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1605,7 +1670,7 @@
         <v>30024</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1613,7 +1678,7 @@
         <v>30025</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1621,7 +1686,7 @@
         <v>30026</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1629,7 +1694,7 @@
         <v>30027</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1637,7 +1702,7 @@
         <v>30028</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1645,7 +1710,7 @@
         <v>30029</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1653,7 +1718,7 @@
         <v>30030</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1661,7 +1726,7 @@
         <v>30031</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1669,7 +1734,7 @@
         <v>30032</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1677,7 +1742,7 @@
         <v>30033</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1685,7 +1750,7 @@
         <v>30034</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1758,7 @@
         <v>30035</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1701,7 +1766,7 @@
         <v>30036</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1709,7 +1774,7 @@
         <v>30037</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1782,7 @@
         <v>30038</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1725,7 +1790,7 @@
         <v>30039</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1733,7 +1798,7 @@
         <v>30040</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1741,7 +1806,7 @@
         <v>30041</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1749,7 +1814,7 @@
         <v>30042</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1757,7 +1822,7 @@
         <v>30043</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1765,7 +1830,7 @@
         <v>30044</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1773,7 +1838,7 @@
         <v>30045</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1781,7 +1846,7 @@
         <v>30046</v>
       </c>
       <c r="C47" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1789,7 +1854,7 @@
         <v>30047</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1797,7 +1862,7 @@
         <v>30048</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1805,7 +1870,7 @@
         <v>30049</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:3" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
@@ -1813,7 +1878,7 @@
         <v>30050</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1821,7 +1886,7 @@
         <v>30051</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1829,7 +1894,7 @@
         <v>30052</v>
       </c>
       <c r="C53" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1837,7 +1902,7 @@
         <v>30053</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1845,7 +1910,7 @@
         <v>30054</v>
       </c>
       <c r="C55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1853,7 +1918,7 @@
         <v>30055</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1861,7 +1926,7 @@
         <v>30056</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1869,7 +1934,7 @@
         <v>30057</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1877,7 +1942,7 @@
         <v>30058</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1885,7 +1950,7 @@
         <v>30059</v>
       </c>
       <c r="C60" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1893,7 +1958,7 @@
         <v>30060</v>
       </c>
       <c r="C61" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1901,7 +1966,7 @@
         <v>30061</v>
       </c>
       <c r="C62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1909,7 +1974,7 @@
         <v>30062</v>
       </c>
       <c r="C63" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1917,7 +1982,7 @@
         <v>30063</v>
       </c>
       <c r="C64" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1925,7 +1990,7 @@
         <v>30064</v>
       </c>
       <c r="C65" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1933,7 +1998,7 @@
         <v>30065</v>
       </c>
       <c r="C66" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1941,7 +2006,7 @@
         <v>30066</v>
       </c>
       <c r="C67" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1949,7 +2014,7 @@
         <v>30067</v>
       </c>
       <c r="C68" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1957,7 +2022,7 @@
         <v>30068</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1965,7 +2030,7 @@
         <v>30069</v>
       </c>
       <c r="C70" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1973,7 +2038,7 @@
         <v>30070</v>
       </c>
       <c r="C71" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1981,7 +2046,7 @@
         <v>30071</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1989,7 +2054,7 @@
         <v>30072</v>
       </c>
       <c r="C73" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1997,7 +2062,7 @@
         <v>30073</v>
       </c>
       <c r="C74" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2005,7 +2070,7 @@
         <v>30074</v>
       </c>
       <c r="C75" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2013,7 +2078,7 @@
         <v>30075</v>
       </c>
       <c r="C76" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2021,7 +2086,7 @@
         <v>30076</v>
       </c>
       <c r="C77" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2029,7 +2094,7 @@
         <v>30077</v>
       </c>
       <c r="C78" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2037,7 +2102,7 @@
         <v>30078</v>
       </c>
       <c r="C79" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2045,7 +2110,7 @@
         <v>30079</v>
       </c>
       <c r="C80" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2118,7 @@
         <v>30080</v>
       </c>
       <c r="C81" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2061,7 +2126,7 @@
         <v>30081</v>
       </c>
       <c r="C82" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2069,7 +2134,7 @@
         <v>30082</v>
       </c>
       <c r="C83" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2077,7 +2142,7 @@
         <v>30083</v>
       </c>
       <c r="C84" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2085,7 +2150,7 @@
         <v>30084</v>
       </c>
       <c r="C85" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2093,7 +2158,7 @@
         <v>30085</v>
       </c>
       <c r="C86" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2101,7 +2166,7 @@
         <v>30086</v>
       </c>
       <c r="C87" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2109,7 +2174,7 @@
         <v>30087</v>
       </c>
       <c r="C88" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2117,7 +2182,7 @@
         <v>30088</v>
       </c>
       <c r="C89" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2125,7 +2190,7 @@
         <v>30089</v>
       </c>
       <c r="C90" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2133,7 +2198,7 @@
         <v>30090</v>
       </c>
       <c r="C91" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2141,7 +2206,7 @@
         <v>30091</v>
       </c>
       <c r="C92" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2149,7 +2214,7 @@
         <v>30092</v>
       </c>
       <c r="C93" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2157,7 +2222,7 @@
         <v>30093</v>
       </c>
       <c r="C94" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2165,7 +2230,7 @@
         <v>30094</v>
       </c>
       <c r="C95" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2173,7 +2238,7 @@
         <v>30095</v>
       </c>
       <c r="C96" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2181,7 +2246,7 @@
         <v>30096</v>
       </c>
       <c r="C97" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2189,7 +2254,7 @@
         <v>30097</v>
       </c>
       <c r="C98" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2197,7 +2262,7 @@
         <v>30098</v>
       </c>
       <c r="C99" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2205,7 +2270,7 @@
         <v>30099</v>
       </c>
       <c r="C100" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:12" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
@@ -2213,7 +2278,7 @@
         <v>30100</v>
       </c>
       <c r="C101" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:12" collapsed="1" x14ac:dyDescent="0.3">
@@ -2221,25 +2286,25 @@
         <v>30101</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D102" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E102" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G102">
         <v>10</v>
       </c>
       <c r="K102" t="s">
+        <v>51</v>
+      </c>
+      <c r="L102" t="s">
         <v>54</v>
-      </c>
-      <c r="L102" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="103" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2247,7 +2312,7 @@
         <v>30102</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2255,7 +2320,7 @@
         <v>30103</v>
       </c>
       <c r="C104" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2263,7 +2328,7 @@
         <v>30104</v>
       </c>
       <c r="C105" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2271,7 +2336,7 @@
         <v>30105</v>
       </c>
       <c r="C106" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2279,7 +2344,7 @@
         <v>30106</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2287,7 +2352,7 @@
         <v>30107</v>
       </c>
       <c r="C108" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2295,7 +2360,7 @@
         <v>30108</v>
       </c>
       <c r="C109" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2303,7 +2368,7 @@
         <v>30109</v>
       </c>
       <c r="C110" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2311,7 +2376,7 @@
         <v>30110</v>
       </c>
       <c r="C111" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2319,7 +2384,7 @@
         <v>30111</v>
       </c>
       <c r="C112" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="113" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2327,7 +2392,7 @@
         <v>30112</v>
       </c>
       <c r="C113" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2335,7 +2400,7 @@
         <v>30113</v>
       </c>
       <c r="C114" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2343,7 +2408,7 @@
         <v>30114</v>
       </c>
       <c r="C115" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="116" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2351,7 +2416,7 @@
         <v>30115</v>
       </c>
       <c r="C116" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="117" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2424,7 @@
         <v>30116</v>
       </c>
       <c r="C117" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="118" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2367,7 +2432,7 @@
         <v>30117</v>
       </c>
       <c r="C118" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2375,7 +2440,7 @@
         <v>30118</v>
       </c>
       <c r="C119" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2383,7 +2448,7 @@
         <v>30119</v>
       </c>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2391,7 +2456,7 @@
         <v>30120</v>
       </c>
       <c r="C121" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2399,7 +2464,7 @@
         <v>30121</v>
       </c>
       <c r="C122" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="123" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2407,7 +2472,7 @@
         <v>30122</v>
       </c>
       <c r="C123" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2415,7 +2480,7 @@
         <v>30123</v>
       </c>
       <c r="C124" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2423,7 +2488,7 @@
         <v>30124</v>
       </c>
       <c r="C125" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2431,7 +2496,7 @@
         <v>30125</v>
       </c>
       <c r="C126" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="127" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2439,7 +2504,7 @@
         <v>30126</v>
       </c>
       <c r="C127" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2447,7 +2512,7 @@
         <v>30127</v>
       </c>
       <c r="C128" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2455,7 +2520,7 @@
         <v>30128</v>
       </c>
       <c r="C129" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2463,7 +2528,7 @@
         <v>30129</v>
       </c>
       <c r="C130" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="131" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2471,7 +2536,7 @@
         <v>30130</v>
       </c>
       <c r="C131" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2479,7 +2544,7 @@
         <v>30131</v>
       </c>
       <c r="C132" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="133" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2487,7 +2552,7 @@
         <v>30132</v>
       </c>
       <c r="C133" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="134" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2495,7 +2560,7 @@
         <v>30133</v>
       </c>
       <c r="C134" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="135" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2503,7 +2568,7 @@
         <v>30134</v>
       </c>
       <c r="C135" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="136" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2576,7 @@
         <v>30135</v>
       </c>
       <c r="C136" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="137" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2519,7 +2584,7 @@
         <v>30136</v>
       </c>
       <c r="C137" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="138" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2527,7 +2592,7 @@
         <v>30137</v>
       </c>
       <c r="C138" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="139" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2535,7 +2600,7 @@
         <v>30138</v>
       </c>
       <c r="C139" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="140" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2543,7 +2608,7 @@
         <v>30139</v>
       </c>
       <c r="C140" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="141" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2551,7 +2616,7 @@
         <v>30140</v>
       </c>
       <c r="C141" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="142" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2559,7 +2624,7 @@
         <v>30141</v>
       </c>
       <c r="C142" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="143" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2567,7 +2632,7 @@
         <v>30142</v>
       </c>
       <c r="C143" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2575,7 +2640,7 @@
         <v>30143</v>
       </c>
       <c r="C144" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="145" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2583,7 +2648,7 @@
         <v>30144</v>
       </c>
       <c r="C145" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2591,7 +2656,7 @@
         <v>30145</v>
       </c>
       <c r="C146" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="147" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2599,7 +2664,7 @@
         <v>30146</v>
       </c>
       <c r="C147" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="148" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2607,7 +2672,7 @@
         <v>30147</v>
       </c>
       <c r="C148" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="149" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2615,7 +2680,7 @@
         <v>30148</v>
       </c>
       <c r="C149" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="150" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2623,7 +2688,7 @@
         <v>30149</v>
       </c>
       <c r="C150" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="151" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2631,7 +2696,7 @@
         <v>30150</v>
       </c>
       <c r="C151" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="152" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2639,7 +2704,7 @@
         <v>30151</v>
       </c>
       <c r="C152" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="153" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2647,7 +2712,7 @@
         <v>30152</v>
       </c>
       <c r="C153" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2655,7 +2720,7 @@
         <v>30153</v>
       </c>
       <c r="C154" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="155" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2663,7 +2728,7 @@
         <v>30154</v>
       </c>
       <c r="C155" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="156" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2671,7 +2736,7 @@
         <v>30155</v>
       </c>
       <c r="C156" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="157" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2679,7 +2744,7 @@
         <v>30156</v>
       </c>
       <c r="C157" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="158" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2687,7 +2752,7 @@
         <v>30157</v>
       </c>
       <c r="C158" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="159" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2695,7 +2760,7 @@
         <v>30158</v>
       </c>
       <c r="C159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="160" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2703,7 +2768,7 @@
         <v>30159</v>
       </c>
       <c r="C160" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="161" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2711,7 +2776,7 @@
         <v>30160</v>
       </c>
       <c r="C161" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="162" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2719,7 +2784,7 @@
         <v>30161</v>
       </c>
       <c r="C162" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="163" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2727,7 +2792,7 @@
         <v>30162</v>
       </c>
       <c r="C163" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2735,7 +2800,7 @@
         <v>30163</v>
       </c>
       <c r="C164" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="165" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2743,7 +2808,7 @@
         <v>30164</v>
       </c>
       <c r="C165" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2751,7 +2816,7 @@
         <v>30165</v>
       </c>
       <c r="C166" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="167" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2759,7 +2824,7 @@
         <v>30166</v>
       </c>
       <c r="C167" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="168" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2832,7 @@
         <v>30167</v>
       </c>
       <c r="C168" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="169" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2840,7 @@
         <v>30168</v>
       </c>
       <c r="C169" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="170" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2783,7 +2848,7 @@
         <v>30169</v>
       </c>
       <c r="C170" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="171" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2791,7 +2856,7 @@
         <v>30170</v>
       </c>
       <c r="C171" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="172" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2799,7 +2864,7 @@
         <v>30171</v>
       </c>
       <c r="C172" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="173" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2807,7 +2872,7 @@
         <v>30172</v>
       </c>
       <c r="C173" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="174" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2815,7 +2880,7 @@
         <v>30173</v>
       </c>
       <c r="C174" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2823,7 +2888,7 @@
         <v>30174</v>
       </c>
       <c r="C175" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="176" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2831,7 +2896,7 @@
         <v>30175</v>
       </c>
       <c r="C176" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="177" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2839,7 +2904,7 @@
         <v>30176</v>
       </c>
       <c r="C177" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="178" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2912,7 @@
         <v>30177</v>
       </c>
       <c r="C178" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="179" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2855,7 +2920,7 @@
         <v>30178</v>
       </c>
       <c r="C179" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="180" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2863,7 +2928,7 @@
         <v>30179</v>
       </c>
       <c r="C180" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2871,7 +2936,7 @@
         <v>30180</v>
       </c>
       <c r="C181" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="182" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2879,7 +2944,7 @@
         <v>30181</v>
       </c>
       <c r="C182" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="183" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2887,7 +2952,7 @@
         <v>30182</v>
       </c>
       <c r="C183" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="184" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2895,7 +2960,7 @@
         <v>30183</v>
       </c>
       <c r="C184" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="185" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2903,7 +2968,7 @@
         <v>30184</v>
       </c>
       <c r="C185" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="186" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2911,7 +2976,7 @@
         <v>30185</v>
       </c>
       <c r="C186" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="187" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2919,7 +2984,7 @@
         <v>30186</v>
       </c>
       <c r="C187" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="188" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2927,7 +2992,7 @@
         <v>30187</v>
       </c>
       <c r="C188" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="189" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2935,7 +3000,7 @@
         <v>30188</v>
       </c>
       <c r="C189" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="190" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2943,7 +3008,7 @@
         <v>30189</v>
       </c>
       <c r="C190" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="191" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2951,7 +3016,7 @@
         <v>30190</v>
       </c>
       <c r="C191" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="192" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2959,7 +3024,7 @@
         <v>30191</v>
       </c>
       <c r="C192" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="193" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2967,7 +3032,7 @@
         <v>30192</v>
       </c>
       <c r="C193" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="194" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2975,7 +3040,7 @@
         <v>30193</v>
       </c>
       <c r="C194" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2983,7 +3048,7 @@
         <v>30194</v>
       </c>
       <c r="C195" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="196" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2991,7 +3056,7 @@
         <v>30195</v>
       </c>
       <c r="C196" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="197" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2999,7 +3064,7 @@
         <v>30196</v>
       </c>
       <c r="C197" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="198" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3007,7 +3072,7 @@
         <v>30197</v>
       </c>
       <c r="C198" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="199" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3015,7 +3080,7 @@
         <v>30198</v>
       </c>
       <c r="C199" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="200" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3023,7 +3088,7 @@
         <v>30199</v>
       </c>
       <c r="C200" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="201" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3031,7 +3096,7 @@
         <v>30200</v>
       </c>
       <c r="C201" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="202" spans="1:11" collapsed="1" x14ac:dyDescent="0.3">
@@ -3039,16 +3104,16 @@
         <v>30201</v>
       </c>
       <c r="B202" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C202" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D202" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F202" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G202">
         <v>3</v>
@@ -3060,7 +3125,7 @@
         <v>2</v>
       </c>
       <c r="K202" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="203" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3563,13 +3628,13 @@
         <v>30301</v>
       </c>
       <c r="B302" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C302" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D302" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G302">
         <v>1</v>
@@ -4084,10 +4149,10 @@
         <v>15</v>
       </c>
       <c r="C402" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D402" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G402">
         <v>1</v>
@@ -7992,9 +8057,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Ark4"/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -8014,16 +8079,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -8036,10 +8101,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>

</xml_diff>

<commit_message>
Change in Exel list
</commit_message>
<xml_diff>
--- a/Documentation/Mobs, NPC, Items, mm.xlsx
+++ b/Documentation/Mobs, NPC, Items, mm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="Denne_projektmappe" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Mobs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -74,15 +74,6 @@
   </si>
   <si>
     <t>Human</t>
-  </si>
-  <si>
-    <t>Briggand</t>
-  </si>
-  <si>
-    <t>Club</t>
-  </si>
-  <si>
-    <t>Stun</t>
   </si>
   <si>
     <t>Gold Drop</t>
@@ -213,13 +204,48 @@
   <si>
     <t>The Iron Daggers Head Quarters.</t>
   </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Defence</t>
+  </si>
+  <si>
+    <t>ExpReward</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>knife</t>
+  </si>
+  <si>
+    <t>Steal</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -247,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -256,6 +282,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,68 +618,83 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -668,20 +710,29 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -689,88 +740,101 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
+        <v>66</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10003</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10004</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10005</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10006</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10007</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10008</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10009</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10010</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10011</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10012</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10013</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10014</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10015</v>
       </c>
@@ -997,6 +1061,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1022,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1034,7 +1099,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -1055,16 +1120,16 @@
         <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1358,34 +1423,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1393,22 +1458,22 @@
         <v>30001</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1417,10 +1482,10 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1429,7 +1494,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1437,7 +1502,7 @@
         <v>30003</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1445,7 +1510,7 @@
         <v>30004</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1453,7 +1518,7 @@
         <v>30005</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1461,7 +1526,7 @@
         <v>30006</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1469,7 +1534,7 @@
         <v>30007</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1477,7 +1542,7 @@
         <v>30008</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="13.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1485,7 +1550,7 @@
         <v>30009</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1493,7 +1558,7 @@
         <v>30010</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1501,7 +1566,7 @@
         <v>30011</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1509,7 +1574,7 @@
         <v>30012</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1517,7 +1582,7 @@
         <v>30013</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1525,7 +1590,7 @@
         <v>30014</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1533,7 +1598,7 @@
         <v>30015</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1541,7 +1606,7 @@
         <v>30016</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1549,7 +1614,7 @@
         <v>30017</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1557,7 +1622,7 @@
         <v>30018</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1565,7 +1630,7 @@
         <v>30019</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1638,7 @@
         <v>30020</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1646,7 @@
         <v>30021</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1589,7 +1654,7 @@
         <v>30022</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1597,7 +1662,7 @@
         <v>30023</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1605,7 +1670,7 @@
         <v>30024</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1613,7 +1678,7 @@
         <v>30025</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1621,7 +1686,7 @@
         <v>30026</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1629,7 +1694,7 @@
         <v>30027</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1637,7 +1702,7 @@
         <v>30028</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1645,7 +1710,7 @@
         <v>30029</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1653,7 +1718,7 @@
         <v>30030</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1661,7 +1726,7 @@
         <v>30031</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1669,7 +1734,7 @@
         <v>30032</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1677,7 +1742,7 @@
         <v>30033</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1685,7 +1750,7 @@
         <v>30034</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1758,7 @@
         <v>30035</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1701,7 +1766,7 @@
         <v>30036</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1709,7 +1774,7 @@
         <v>30037</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1782,7 @@
         <v>30038</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1725,7 +1790,7 @@
         <v>30039</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1733,7 +1798,7 @@
         <v>30040</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1741,7 +1806,7 @@
         <v>30041</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1749,7 +1814,7 @@
         <v>30042</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1757,7 +1822,7 @@
         <v>30043</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1765,7 +1830,7 @@
         <v>30044</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1773,7 +1838,7 @@
         <v>30045</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1781,7 +1846,7 @@
         <v>30046</v>
       </c>
       <c r="C47" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1789,7 +1854,7 @@
         <v>30047</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1797,7 +1862,7 @@
         <v>30048</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1805,7 +1870,7 @@
         <v>30049</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:3" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
@@ -1813,7 +1878,7 @@
         <v>30050</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1821,7 +1886,7 @@
         <v>30051</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1829,7 +1894,7 @@
         <v>30052</v>
       </c>
       <c r="C53" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1837,7 +1902,7 @@
         <v>30053</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1845,7 +1910,7 @@
         <v>30054</v>
       </c>
       <c r="C55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1853,7 +1918,7 @@
         <v>30055</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1861,7 +1926,7 @@
         <v>30056</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1869,7 +1934,7 @@
         <v>30057</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1877,7 +1942,7 @@
         <v>30058</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1885,7 +1950,7 @@
         <v>30059</v>
       </c>
       <c r="C60" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1893,7 +1958,7 @@
         <v>30060</v>
       </c>
       <c r="C61" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1901,7 +1966,7 @@
         <v>30061</v>
       </c>
       <c r="C62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1909,7 +1974,7 @@
         <v>30062</v>
       </c>
       <c r="C63" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1917,7 +1982,7 @@
         <v>30063</v>
       </c>
       <c r="C64" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1925,7 +1990,7 @@
         <v>30064</v>
       </c>
       <c r="C65" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1933,7 +1998,7 @@
         <v>30065</v>
       </c>
       <c r="C66" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1941,7 +2006,7 @@
         <v>30066</v>
       </c>
       <c r="C67" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1949,7 +2014,7 @@
         <v>30067</v>
       </c>
       <c r="C68" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1957,7 +2022,7 @@
         <v>30068</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1965,7 +2030,7 @@
         <v>30069</v>
       </c>
       <c r="C70" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1973,7 +2038,7 @@
         <v>30070</v>
       </c>
       <c r="C71" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1981,7 +2046,7 @@
         <v>30071</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1989,7 +2054,7 @@
         <v>30072</v>
       </c>
       <c r="C73" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1997,7 +2062,7 @@
         <v>30073</v>
       </c>
       <c r="C74" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2005,7 +2070,7 @@
         <v>30074</v>
       </c>
       <c r="C75" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2013,7 +2078,7 @@
         <v>30075</v>
       </c>
       <c r="C76" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2021,7 +2086,7 @@
         <v>30076</v>
       </c>
       <c r="C77" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2029,7 +2094,7 @@
         <v>30077</v>
       </c>
       <c r="C78" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2037,7 +2102,7 @@
         <v>30078</v>
       </c>
       <c r="C79" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2045,7 +2110,7 @@
         <v>30079</v>
       </c>
       <c r="C80" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2118,7 @@
         <v>30080</v>
       </c>
       <c r="C81" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2061,7 +2126,7 @@
         <v>30081</v>
       </c>
       <c r="C82" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2069,7 +2134,7 @@
         <v>30082</v>
       </c>
       <c r="C83" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2077,7 +2142,7 @@
         <v>30083</v>
       </c>
       <c r="C84" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2085,7 +2150,7 @@
         <v>30084</v>
       </c>
       <c r="C85" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2093,7 +2158,7 @@
         <v>30085</v>
       </c>
       <c r="C86" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2101,7 +2166,7 @@
         <v>30086</v>
       </c>
       <c r="C87" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2109,7 +2174,7 @@
         <v>30087</v>
       </c>
       <c r="C88" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2117,7 +2182,7 @@
         <v>30088</v>
       </c>
       <c r="C89" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2125,7 +2190,7 @@
         <v>30089</v>
       </c>
       <c r="C90" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2133,7 +2198,7 @@
         <v>30090</v>
       </c>
       <c r="C91" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2141,7 +2206,7 @@
         <v>30091</v>
       </c>
       <c r="C92" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2149,7 +2214,7 @@
         <v>30092</v>
       </c>
       <c r="C93" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2157,7 +2222,7 @@
         <v>30093</v>
       </c>
       <c r="C94" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2165,7 +2230,7 @@
         <v>30094</v>
       </c>
       <c r="C95" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2173,7 +2238,7 @@
         <v>30095</v>
       </c>
       <c r="C96" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2181,7 +2246,7 @@
         <v>30096</v>
       </c>
       <c r="C97" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2189,7 +2254,7 @@
         <v>30097</v>
       </c>
       <c r="C98" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2197,7 +2262,7 @@
         <v>30098</v>
       </c>
       <c r="C99" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2205,7 +2270,7 @@
         <v>30099</v>
       </c>
       <c r="C100" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:12" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
@@ -2213,7 +2278,7 @@
         <v>30100</v>
       </c>
       <c r="C101" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:12" collapsed="1" x14ac:dyDescent="0.3">
@@ -2221,25 +2286,25 @@
         <v>30101</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D102" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E102" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G102">
         <v>10</v>
       </c>
       <c r="K102" t="s">
+        <v>51</v>
+      </c>
+      <c r="L102" t="s">
         <v>54</v>
-      </c>
-      <c r="L102" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="103" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2247,7 +2312,7 @@
         <v>30102</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2255,7 +2320,7 @@
         <v>30103</v>
       </c>
       <c r="C104" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2263,7 +2328,7 @@
         <v>30104</v>
       </c>
       <c r="C105" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2271,7 +2336,7 @@
         <v>30105</v>
       </c>
       <c r="C106" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2279,7 +2344,7 @@
         <v>30106</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2287,7 +2352,7 @@
         <v>30107</v>
       </c>
       <c r="C108" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2295,7 +2360,7 @@
         <v>30108</v>
       </c>
       <c r="C109" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2303,7 +2368,7 @@
         <v>30109</v>
       </c>
       <c r="C110" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2311,7 +2376,7 @@
         <v>30110</v>
       </c>
       <c r="C111" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2319,7 +2384,7 @@
         <v>30111</v>
       </c>
       <c r="C112" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="113" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2327,7 +2392,7 @@
         <v>30112</v>
       </c>
       <c r="C113" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2335,7 +2400,7 @@
         <v>30113</v>
       </c>
       <c r="C114" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2343,7 +2408,7 @@
         <v>30114</v>
       </c>
       <c r="C115" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="116" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2351,7 +2416,7 @@
         <v>30115</v>
       </c>
       <c r="C116" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="117" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2424,7 @@
         <v>30116</v>
       </c>
       <c r="C117" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="118" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2367,7 +2432,7 @@
         <v>30117</v>
       </c>
       <c r="C118" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2375,7 +2440,7 @@
         <v>30118</v>
       </c>
       <c r="C119" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2383,7 +2448,7 @@
         <v>30119</v>
       </c>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2391,7 +2456,7 @@
         <v>30120</v>
       </c>
       <c r="C121" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2399,7 +2464,7 @@
         <v>30121</v>
       </c>
       <c r="C122" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="123" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2407,7 +2472,7 @@
         <v>30122</v>
       </c>
       <c r="C123" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2415,7 +2480,7 @@
         <v>30123</v>
       </c>
       <c r="C124" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2423,7 +2488,7 @@
         <v>30124</v>
       </c>
       <c r="C125" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2431,7 +2496,7 @@
         <v>30125</v>
       </c>
       <c r="C126" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="127" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2439,7 +2504,7 @@
         <v>30126</v>
       </c>
       <c r="C127" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2447,7 +2512,7 @@
         <v>30127</v>
       </c>
       <c r="C128" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2455,7 +2520,7 @@
         <v>30128</v>
       </c>
       <c r="C129" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2463,7 +2528,7 @@
         <v>30129</v>
       </c>
       <c r="C130" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="131" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2471,7 +2536,7 @@
         <v>30130</v>
       </c>
       <c r="C131" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2479,7 +2544,7 @@
         <v>30131</v>
       </c>
       <c r="C132" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="133" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2487,7 +2552,7 @@
         <v>30132</v>
       </c>
       <c r="C133" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="134" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2495,7 +2560,7 @@
         <v>30133</v>
       </c>
       <c r="C134" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="135" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2503,7 +2568,7 @@
         <v>30134</v>
       </c>
       <c r="C135" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="136" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2576,7 @@
         <v>30135</v>
       </c>
       <c r="C136" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="137" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2519,7 +2584,7 @@
         <v>30136</v>
       </c>
       <c r="C137" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="138" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2527,7 +2592,7 @@
         <v>30137</v>
       </c>
       <c r="C138" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="139" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2535,7 +2600,7 @@
         <v>30138</v>
       </c>
       <c r="C139" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="140" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2543,7 +2608,7 @@
         <v>30139</v>
       </c>
       <c r="C140" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="141" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2551,7 +2616,7 @@
         <v>30140</v>
       </c>
       <c r="C141" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="142" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2559,7 +2624,7 @@
         <v>30141</v>
       </c>
       <c r="C142" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="143" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2567,7 +2632,7 @@
         <v>30142</v>
       </c>
       <c r="C143" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2575,7 +2640,7 @@
         <v>30143</v>
       </c>
       <c r="C144" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="145" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2583,7 +2648,7 @@
         <v>30144</v>
       </c>
       <c r="C145" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2591,7 +2656,7 @@
         <v>30145</v>
       </c>
       <c r="C146" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="147" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2599,7 +2664,7 @@
         <v>30146</v>
       </c>
       <c r="C147" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="148" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2607,7 +2672,7 @@
         <v>30147</v>
       </c>
       <c r="C148" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="149" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2615,7 +2680,7 @@
         <v>30148</v>
       </c>
       <c r="C149" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="150" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2623,7 +2688,7 @@
         <v>30149</v>
       </c>
       <c r="C150" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="151" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2631,7 +2696,7 @@
         <v>30150</v>
       </c>
       <c r="C151" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="152" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2639,7 +2704,7 @@
         <v>30151</v>
       </c>
       <c r="C152" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="153" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2647,7 +2712,7 @@
         <v>30152</v>
       </c>
       <c r="C153" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2655,7 +2720,7 @@
         <v>30153</v>
       </c>
       <c r="C154" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="155" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2663,7 +2728,7 @@
         <v>30154</v>
       </c>
       <c r="C155" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="156" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2671,7 +2736,7 @@
         <v>30155</v>
       </c>
       <c r="C156" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="157" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2679,7 +2744,7 @@
         <v>30156</v>
       </c>
       <c r="C157" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="158" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2687,7 +2752,7 @@
         <v>30157</v>
       </c>
       <c r="C158" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="159" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2695,7 +2760,7 @@
         <v>30158</v>
       </c>
       <c r="C159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="160" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2703,7 +2768,7 @@
         <v>30159</v>
       </c>
       <c r="C160" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="161" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2711,7 +2776,7 @@
         <v>30160</v>
       </c>
       <c r="C161" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="162" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2719,7 +2784,7 @@
         <v>30161</v>
       </c>
       <c r="C162" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="163" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2727,7 +2792,7 @@
         <v>30162</v>
       </c>
       <c r="C163" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2735,7 +2800,7 @@
         <v>30163</v>
       </c>
       <c r="C164" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="165" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2743,7 +2808,7 @@
         <v>30164</v>
       </c>
       <c r="C165" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2751,7 +2816,7 @@
         <v>30165</v>
       </c>
       <c r="C166" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="167" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2759,7 +2824,7 @@
         <v>30166</v>
       </c>
       <c r="C167" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="168" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2832,7 @@
         <v>30167</v>
       </c>
       <c r="C168" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="169" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2840,7 @@
         <v>30168</v>
       </c>
       <c r="C169" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="170" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2783,7 +2848,7 @@
         <v>30169</v>
       </c>
       <c r="C170" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="171" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2791,7 +2856,7 @@
         <v>30170</v>
       </c>
       <c r="C171" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="172" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2799,7 +2864,7 @@
         <v>30171</v>
       </c>
       <c r="C172" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="173" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2807,7 +2872,7 @@
         <v>30172</v>
       </c>
       <c r="C173" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="174" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2815,7 +2880,7 @@
         <v>30173</v>
       </c>
       <c r="C174" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2823,7 +2888,7 @@
         <v>30174</v>
       </c>
       <c r="C175" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="176" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2831,7 +2896,7 @@
         <v>30175</v>
       </c>
       <c r="C176" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="177" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2839,7 +2904,7 @@
         <v>30176</v>
       </c>
       <c r="C177" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="178" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2912,7 @@
         <v>30177</v>
       </c>
       <c r="C178" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="179" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2855,7 +2920,7 @@
         <v>30178</v>
       </c>
       <c r="C179" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="180" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2863,7 +2928,7 @@
         <v>30179</v>
       </c>
       <c r="C180" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2871,7 +2936,7 @@
         <v>30180</v>
       </c>
       <c r="C181" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="182" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2879,7 +2944,7 @@
         <v>30181</v>
       </c>
       <c r="C182" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="183" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2887,7 +2952,7 @@
         <v>30182</v>
       </c>
       <c r="C183" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="184" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2895,7 +2960,7 @@
         <v>30183</v>
       </c>
       <c r="C184" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="185" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2903,7 +2968,7 @@
         <v>30184</v>
       </c>
       <c r="C185" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="186" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2911,7 +2976,7 @@
         <v>30185</v>
       </c>
       <c r="C186" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="187" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2919,7 +2984,7 @@
         <v>30186</v>
       </c>
       <c r="C187" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="188" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2927,7 +2992,7 @@
         <v>30187</v>
       </c>
       <c r="C188" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="189" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2935,7 +3000,7 @@
         <v>30188</v>
       </c>
       <c r="C189" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="190" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2943,7 +3008,7 @@
         <v>30189</v>
       </c>
       <c r="C190" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="191" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2951,7 +3016,7 @@
         <v>30190</v>
       </c>
       <c r="C191" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="192" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2959,7 +3024,7 @@
         <v>30191</v>
       </c>
       <c r="C192" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="193" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2967,7 +3032,7 @@
         <v>30192</v>
       </c>
       <c r="C193" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="194" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2975,7 +3040,7 @@
         <v>30193</v>
       </c>
       <c r="C194" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2983,7 +3048,7 @@
         <v>30194</v>
       </c>
       <c r="C195" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="196" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2991,7 +3056,7 @@
         <v>30195</v>
       </c>
       <c r="C196" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="197" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2999,7 +3064,7 @@
         <v>30196</v>
       </c>
       <c r="C197" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="198" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3007,7 +3072,7 @@
         <v>30197</v>
       </c>
       <c r="C198" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="199" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3015,7 +3080,7 @@
         <v>30198</v>
       </c>
       <c r="C199" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="200" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3023,7 +3088,7 @@
         <v>30199</v>
       </c>
       <c r="C200" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="201" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3031,7 +3096,7 @@
         <v>30200</v>
       </c>
       <c r="C201" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="202" spans="1:11" collapsed="1" x14ac:dyDescent="0.3">
@@ -3039,16 +3104,16 @@
         <v>30201</v>
       </c>
       <c r="B202" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C202" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D202" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F202" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G202">
         <v>3</v>
@@ -3060,7 +3125,7 @@
         <v>2</v>
       </c>
       <c r="K202" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="203" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3563,13 +3628,13 @@
         <v>30301</v>
       </c>
       <c r="B302" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C302" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D302" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G302">
         <v>1</v>
@@ -4084,10 +4149,10 @@
         <v>15</v>
       </c>
       <c r="C402" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D402" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G402">
         <v>1</v>
@@ -7992,9 +8057,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Ark4"/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -8014,16 +8079,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -8036,10 +8101,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>

</xml_diff>